<commit_message>
Added function 93 95 96
</commit_message>
<xml_diff>
--- a/inst/excel_files/waveform4R.xlsx
+++ b/inst/excel_files/waveform4R.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.ripamonti\Documents\Scaphoideus.titanus_2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Documents/001_WORK/CNR/Rwaves/inst/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C7D5C0-2A6B-4D41-8813-C478332BF5BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="9168" activeTab="2"/>
+    <workbookView xWindow="-28240" yWindow="460" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stylet+_waves-codes" sheetId="2" r:id="rId1"/>
     <sheet name="Variables" sheetId="1" r:id="rId2"/>
-    <sheet name="Variables_conc" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="171">
   <si>
     <t>n_Np</t>
   </si>
@@ -184,12 +181,6 @@
     <t>1, 4, 5, 8, 9</t>
   </si>
   <si>
-    <t>n_phloemph</t>
-  </si>
-  <si>
-    <t>Number of phloem phases</t>
-  </si>
-  <si>
     <t>n_sE2</t>
   </si>
   <si>
@@ -274,103 +265,286 @@
     <t>C</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>[11]</t>
+  </si>
+  <si>
+    <t>[12]</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Stylets pathway phase</t>
+  </si>
+  <si>
+    <t>Wave-name_S.titanus</t>
+  </si>
+  <si>
+    <t>Flat-interruption during ingestion</t>
+  </si>
+  <si>
+    <t>End of recording</t>
+  </si>
+  <si>
+    <t>Derailed stylets pathway</t>
+  </si>
+  <si>
+    <t>Active ingestion</t>
+  </si>
+  <si>
+    <t>Non probing</t>
+  </si>
+  <si>
+    <t>Hat_spikes-interruption during ingestion</t>
+  </si>
+  <si>
+    <t>Wave-number associated</t>
+  </si>
+  <si>
+    <t>formula (number=waveforms)</t>
+  </si>
+  <si>
+    <t>number of probes</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>total number of 7</t>
+  </si>
+  <si>
+    <t>total duration of 7</t>
+  </si>
+  <si>
+    <t>total duration of 2</t>
+  </si>
+  <si>
+    <t>total duration of 6</t>
+  </si>
+  <si>
+    <t>everything between two "1" waves is a probe; it is possible that at the end of the recording a probe is still ongoing, so there is no "1" wave after</t>
+  </si>
+  <si>
+    <t>total recording time - total duration of 1</t>
+  </si>
+  <si>
+    <t>duration of the 2nd "1" wave</t>
+  </si>
+  <si>
+    <t>total number of "1"</t>
+  </si>
+  <si>
+    <t>total duration of "1"</t>
+  </si>
+  <si>
+    <t>total number of "4"</t>
+  </si>
+  <si>
+    <t>total duration of "4"</t>
+  </si>
+  <si>
+    <t>number of "5" longer than 10 minutes</t>
+  </si>
+  <si>
+    <t>(total duration of "5")/(total duration of probing time)</t>
+  </si>
+  <si>
+    <t>total duration of "3", "4" and "5"</t>
+  </si>
+  <si>
+    <t>(total duration of probing time) - (total duration of "3", "4" and "5")</t>
+  </si>
+  <si>
+    <t>end of EPG record - (time from the 1st "4")</t>
+  </si>
+  <si>
+    <t>(total duration of "4"/total duration of the probing time)*100</t>
+  </si>
+  <si>
+    <t>(total duration of 2/total duration of the probing time)*100</t>
+  </si>
+  <si>
+    <t>(total duration of 6/total duration of the probing time)*100</t>
+  </si>
+  <si>
+    <t>(total duration of 7/total duration of the probing time)*100</t>
+  </si>
+  <si>
+    <t>%probtimeinE</t>
+  </si>
+  <si>
+    <t>% of probing time spent in E2</t>
+  </si>
+  <si>
+    <t>% of probing time spent in E</t>
+  </si>
+  <si>
+    <t>((total duration of "3","4" and "5")/(total duration of the probing time))*100</t>
+  </si>
+  <si>
+    <t>%probtimeinE2</t>
+  </si>
+  <si>
+    <t>(total duration of "5"/total duration of the probing time)*100</t>
+  </si>
+  <si>
+    <t>119E</t>
+  </si>
+  <si>
+    <t>n_E2</t>
+  </si>
+  <si>
+    <t>Number of E2</t>
+  </si>
+  <si>
+    <t>s_E2</t>
+  </si>
+  <si>
+    <t>Total duration of E2</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 5, 9</t>
+  </si>
+  <si>
+    <t>a_E2</t>
+  </si>
+  <si>
+    <t>Mean duration of E2</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>s_longestE2</t>
+  </si>
+  <si>
+    <t>Duration of the longest E2</t>
+  </si>
+  <si>
+    <t>Phloem acceptability</t>
+  </si>
+  <si>
+    <t>total number of "5"</t>
+  </si>
+  <si>
+    <t>N.B: waves [11] and [12], called brief interruptions, don't interrupt the whole wave in which they are present. i.e. 10 min of waveform "5" in which there are present several [12] interruptions (20), count as one "5" waveform that lasts 10 min. Every other waves interrupt "5" (i.e. "2", "6", "1")</t>
+  </si>
+  <si>
+    <t>total duration of "5"</t>
+  </si>
+  <si>
+    <t>mean duration of one "5"</t>
+  </si>
+  <si>
+    <t>duration of the longest "5"</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>f115_5</t>
+  </si>
+  <si>
+    <t>ff115_4</t>
+  </si>
+  <si>
+    <t>ff1_4</t>
+  </si>
+  <si>
+    <t>ff2_4</t>
+  </si>
+  <si>
+    <t>ff2_5</t>
+  </si>
+  <si>
+    <t>ff91/ff24</t>
+  </si>
+  <si>
     <t>E1</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>[11]</t>
-  </si>
-  <si>
-    <t>[12]</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>Stylets pathway phase</t>
-  </si>
-  <si>
-    <t>Phloem phase</t>
-  </si>
-  <si>
-    <t>Wave-name_S.titanus</t>
-  </si>
-  <si>
-    <t>Flat-interruption during ingestion</t>
-  </si>
-  <si>
-    <t>End of recording</t>
-  </si>
-  <si>
-    <t>Derailed stylets pathway</t>
-  </si>
-  <si>
-    <t>Active ingestion</t>
-  </si>
-  <si>
-    <t>Non probing</t>
-  </si>
-  <si>
-    <t>Hat_spikes-interruption during ingestion</t>
-  </si>
-  <si>
-    <t>Wave-number associated</t>
-  </si>
-  <si>
-    <t>formula (number=waveforms)</t>
-  </si>
-  <si>
-    <t>number of probes</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>total number of 7</t>
-  </si>
-  <si>
-    <t>total duration of 7</t>
-  </si>
-  <si>
-    <t>total duration of 2</t>
-  </si>
-  <si>
-    <t>total duration of 6</t>
-  </si>
-  <si>
-    <t>(total duration of 7/total duration of the recording)*100</t>
-  </si>
-  <si>
-    <t>(total duration of 2/total duration of the recording)*100</t>
-  </si>
-  <si>
-    <t>(total duration of 6/total duration of the recording)*100</t>
-  </si>
-  <si>
-    <t>everything between two "1" waves is a probe; it is possible that at the end of the recording a probe is still ongoing, so there is no "1" wave after</t>
-  </si>
-  <si>
-    <t>total recording time - total duration of 1</t>
-  </si>
-  <si>
-    <t>duration of the 2nd "1" wave</t>
-  </si>
-  <si>
-    <t>total number of "1"</t>
-  </si>
-  <si>
-    <t>total duration of "1"</t>
+    <t>Salivation in phloem phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passive ingestion in phloem phase </t>
+  </si>
+  <si>
+    <t>functions in Rwaves</t>
+  </si>
+  <si>
+    <t>removed</t>
+  </si>
+  <si>
+    <t>f89_5</t>
+  </si>
+  <si>
+    <t>f90_5</t>
+  </si>
+  <si>
+    <t>mean frequency of 12 during 5</t>
+  </si>
+  <si>
+    <t>% of 12 during 5</t>
+  </si>
+  <si>
+    <t>value [Hz]</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>(number of 12 during phase 5/total time of phase 5(including 12+11))</t>
+  </si>
+  <si>
+    <t>(time passed in 12 during phase 5/ total time of phase 5(including 12+11))*100</t>
+  </si>
+  <si>
+    <t>f1_1</t>
+  </si>
+  <si>
+    <t>f1_7</t>
+  </si>
+  <si>
+    <t>f115_2</t>
+  </si>
+  <si>
+    <t>fr115_7</t>
+  </si>
+  <si>
+    <t>f14</t>
+  </si>
+  <si>
+    <t>f2_1</t>
+  </si>
+  <si>
+    <t>f2_2</t>
+  </si>
+  <si>
+    <t>f24</t>
+  </si>
+  <si>
+    <t>f2_7</t>
+  </si>
+  <si>
+    <t>f3_1</t>
+  </si>
+  <si>
+    <t>filter(max(ff89))</t>
+  </si>
+  <si>
+    <t>CONTROLLARE perché la 5 non dev'essere interrotta dalla 11 e 12 (Fatta da matteo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,15 +571,45 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -422,11 +626,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,11 +655,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -459,41 +701,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Authors and citation"/>
-      <sheetName val="1. Instructions"/>
-      <sheetName val="2. Parameters information"/>
-      <sheetName val="3. Software &amp; Run"/>
-      <sheetName val="4. Raw data"/>
-      <sheetName val="5. Results"/>
-      <sheetName val="Data Processing 1"/>
-      <sheetName val="Data Processing 2bis"/>
-      <sheetName val="Data Processing 2"/>
-      <sheetName val="Data processing 3"/>
-      <sheetName val="S.t. EPG III rev"/>
-      <sheetName val="Events"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -758,116 +965,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10">
         <v>99</v>
       </c>
     </row>
@@ -877,30 +1095,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="35.44140625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="35.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -929,13 +1149,16 @@
         <v>25</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -964,10 +1187,13 @@
         <v>7</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -996,10 +1222,13 @@
         <v>11</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="56" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -1028,10 +1257,13 @@
         <v>16</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>14</v>
       </c>
@@ -1060,13 +1292,16 @@
         <v>28</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="42" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>24</v>
       </c>
@@ -1095,11 +1330,14 @@
         <v>31</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="L6" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>29</v>
       </c>
@@ -1128,42 +1366,48 @@
         <v>34</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+        <v>98</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="12" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
         <v>67</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="J8" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>57</v>
       </c>
@@ -1192,10 +1436,13 @@
         <v>38</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>58</v>
       </c>
@@ -1224,24 +1471,27 @@
         <v>4</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="56" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>115</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>4</v>
@@ -1250,80 +1500,90 @@
         <v>5</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I11" s="2">
         <v>11</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+        <v>113</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="12" customFormat="1" ht="56" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
         <v>116</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="10">
+        <v>11</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>117</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="2">
+      <c r="F13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="7">
         <v>11</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>117</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="2">
-        <v>11</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="J13" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="29" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>75</v>
       </c>
@@ -1351,8 +1611,14 @@
       <c r="I14" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="J14" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>78</v>
       </c>
@@ -1380,17 +1646,25 @@
       <c r="I15" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="J15" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="98" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>89</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>3</v>
@@ -1404,20 +1678,31 @@
       <c r="H16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="I16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="98" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>90</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>3</v>
@@ -1434,22 +1719,31 @@
       <c r="I17" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="J17" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="70" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>125</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>46</v>
@@ -1458,24 +1752,33 @@
         <v>5</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="28" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>10</v>
@@ -1487,340 +1790,322 @@
         <v>5</v>
       </c>
       <c r="H19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I19" s="2">
+        <v>4</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="17" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
+        <v>93</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I20" s="18">
+        <v>10</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="17" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+      <c r="A21" s="18">
+        <v>95</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+      <c r="A22" s="18">
+        <v>96</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>98</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>98</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="J23" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>107</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2" t="s">
+      <c r="G24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>107</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I21" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="I24" s="2">
+        <v>5</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>118</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" s="2">
+      <c r="G25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="2">
         <v>11</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>14</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>24</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>29</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>67</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>57</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
-        <v>58</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>115</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="J25" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+      <c r="A26" s="15">
+        <v>119</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="15">
+        <v>11</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="K26" s="17"/>
+      <c r="L26" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>117</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
-        <v>75</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
-        <v>78</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
-        <v>90</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
-        <v>95</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
-        <v>96</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
-        <v>98</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
-        <v>107</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
+      <c r="C27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>76</v>
+      <c r="E27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="17" customFormat="1" ht="70" x14ac:dyDescent="0.2">
+      <c r="A28" s="16">
+        <v>200</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="17" customFormat="1" ht="70" x14ac:dyDescent="0.2">
+      <c r="A29" s="16">
+        <v>201</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 200 and 201
</commit_message>
<xml_diff>
--- a/inst/excel_files/waveform4R.xlsx
+++ b/inst/excel_files/waveform4R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Documents/001_WORK/CNR/Rwaves/inst/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F08F241-BA72-7840-ABEF-CB5FBBB4F926}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ECA064-30CB-4C44-B926-3F82A54B44F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28240" yWindow="460" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1095,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added 98 and 119E
</commit_message>
<xml_diff>
--- a/inst/excel_files/waveform4R.xlsx
+++ b/inst/excel_files/waveform4R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Documents/001_WORK/CNR/Rwaves/inst/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ECA064-30CB-4C44-B926-3F82A54B44F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D6FDA4-7486-A947-94C8-EE4DBDF2A69F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28240" yWindow="460" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,7 +568,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,6 +605,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -636,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -656,7 +662,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -670,9 +675,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -683,6 +685,15 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1369,38 +1380,38 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="12" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
+    <row r="8" spans="1:12" s="11" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
         <v>67</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="10" t="s">
+      <c r="G8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="11" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1509,38 +1520,38 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="12" customFormat="1" ht="56" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+    <row r="12" spans="1:12" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
         <v>116</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="10" t="s">
+      <c r="G12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <v>11</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="11" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1611,7 +1622,7 @@
       <c r="J14" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="12" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1646,7 +1657,7 @@
       <c r="J15" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L15" s="12" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1684,7 +1695,7 @@
       <c r="K16" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="L16" s="14" t="s">
+      <c r="L16" s="13" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1722,42 +1733,42 @@
       <c r="K17" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="13" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="28" x14ac:dyDescent="0.2">
-      <c r="A18" s="18">
+      <c r="A18" s="16">
         <v>91</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="18" t="s">
+      <c r="G18" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="I18" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="L18" s="12" t="s">
         <v>144</v>
       </c>
       <c r="M18" s="6"/>
@@ -1794,137 +1805,137 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="17" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A20" s="18">
+    <row r="20" spans="1:13" s="15" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="A20" s="16">
         <v>93</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="16">
         <v>10</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="L20" s="17" t="s">
+      <c r="L20" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="17" customFormat="1" ht="42" x14ac:dyDescent="0.2">
-      <c r="A21" s="18">
+    <row r="21" spans="1:13" s="15" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+      <c r="A21" s="16">
         <v>95</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" s="18" t="s">
+      <c r="G21" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="14" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="28" x14ac:dyDescent="0.2">
-      <c r="A22" s="18">
+      <c r="A22" s="16">
         <v>96</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="18" t="s">
+      <c r="G22" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="17" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="56" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="19">
         <v>98</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="G23" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J23" s="20" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1961,143 +1972,152 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="56" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="19">
         <v>118</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2" t="s">
+      <c r="G25" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="19">
         <v>11</v>
       </c>
-      <c r="J25" s="6" t="s">
+      <c r="J25" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="L25" s="12" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="56" x14ac:dyDescent="0.2">
-      <c r="A26" s="18">
+      <c r="A26" s="16">
         <v>119</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="18" t="s">
+      <c r="G26" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I26" s="16">
         <v>11</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="13" t="s">
+      <c r="K26" s="15"/>
+      <c r="L26" s="12" t="s">
         <v>140</v>
       </c>
       <c r="M26" s="6"/>
     </row>
     <row r="27" spans="1:13" ht="70" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="2" t="s">
+      <c r="G27" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J27" s="6" t="s">
+      <c r="I27" s="22"/>
+      <c r="J27" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="17" customFormat="1" ht="70" x14ac:dyDescent="0.2">
-      <c r="A28" s="16">
+    <row r="28" spans="1:13" s="15" customFormat="1" ht="70" x14ac:dyDescent="0.2">
+      <c r="A28" s="17">
         <v>200</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="G28" s="18"/>
+      <c r="H28" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="J28" s="16" t="s">
+      <c r="I28" s="18"/>
+      <c r="J28" s="17" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="17" customFormat="1" ht="70" x14ac:dyDescent="0.2">
-      <c r="A29" s="16">
+    <row r="29" spans="1:13" s="15" customFormat="1" ht="70" x14ac:dyDescent="0.2">
+      <c r="A29" s="17">
         <v>201</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="G29" s="18"/>
+      <c r="H29" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="J29" s="16" t="s">
+      <c r="I29" s="18"/>
+      <c r="J29" s="17" t="s">
         <v>158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the Excel file with formulas
</commit_message>
<xml_diff>
--- a/inst/excel_files/waveform4R.xlsx
+++ b/inst/excel_files/waveform4R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Documents/001_WORK/CNR/Rwaves/inst/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D6FDA4-7486-A947-94C8-EE4DBDF2A69F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6964A7D7-58F9-F947-BD86-E7712A05A0AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28240" yWindow="460" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:J27"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated excel file with formulas
</commit_message>
<xml_diff>
--- a/inst/excel_files/waveform4R.xlsx
+++ b/inst/excel_files/waveform4R.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Documents/001_WORK/CNR/Rwaves/inst/excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.ripamonti\Documents\Scaphoideus.titanus_2019\Rwaves analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6964A7D7-58F9-F947-BD86-E7712A05A0AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28240" yWindow="460" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="9168" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stylet+_waves-codes" sheetId="2" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="180">
   <si>
     <t>n_Np</t>
   </si>
@@ -535,13 +534,43 @@
     <t>f3_1</t>
   </si>
   <si>
-    <t>filter(max(ff89))</t>
+    <t>4, 5</t>
+  </si>
+  <si>
+    <t>t_1sE2.exp</t>
+  </si>
+  <si>
+    <t>Time from 1st probe to 1st sustained E2 (10 minutes)†</t>
+  </si>
+  <si>
+    <t>f109</t>
+  </si>
+  <si>
+    <t>f_added_date</t>
+  </si>
+  <si>
+    <t>t_1E2.exp</t>
+  </si>
+  <si>
+    <t>Time from 1st probe to 1st E2†</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4, 5 </t>
+  </si>
+  <si>
+    <t>f112</t>
+  </si>
+  <si>
+    <t>time to first E2 - first 2 wave</t>
+  </si>
+  <si>
+    <t>time to first sustained E2 - first 2 wave</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -568,7 +597,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -590,24 +619,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -662,6 +673,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -675,28 +687,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -973,21 +967,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -998,7 +992,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1009,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1020,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>147</v>
       </c>
@@ -1031,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>148</v>
       </c>
@@ -1042,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -1053,7 +1047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1064,7 +1058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -1075,7 +1069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -1086,7 +1080,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1103,32 +1097,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="35.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="1"/>
+    <col min="13" max="13" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1165,8 +1159,11 @@
       <c r="L1" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.2">
+      <c r="M1" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1201,7 +1198,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1236,7 +1233,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -1271,7 +1268,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>14</v>
       </c>
@@ -1309,7 +1306,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>24</v>
       </c>
@@ -1345,7 +1342,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>29</v>
       </c>
@@ -1380,42 +1377,42 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="11" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+    <row r="8" spans="1:13" s="12" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
         <v>67</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="G8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>57</v>
       </c>
@@ -1450,7 +1447,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>58</v>
       </c>
@@ -1485,7 +1482,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="56" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>115</v>
       </c>
@@ -1520,42 +1517,42 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
+    <row r="12" spans="1:13" s="12" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>116</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="9" t="s">
+      <c r="G12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="10">
         <v>11</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>117</v>
       </c>
@@ -1591,7 +1588,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="29" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="27" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>75</v>
       </c>
@@ -1622,11 +1619,11 @@
       <c r="J14" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>78</v>
       </c>
@@ -1657,11 +1654,11 @@
       <c r="J15" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="98" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>89</v>
       </c>
@@ -1695,11 +1692,11 @@
       <c r="K16" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="98" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>90</v>
       </c>
@@ -1733,47 +1730,46 @@
       <c r="K17" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="28" x14ac:dyDescent="0.2">
-      <c r="A18" s="16">
+    <row r="18" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
         <v>91</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="16" t="s">
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="L18" s="12" t="s">
+      <c r="L18" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>92</v>
       </c>
@@ -1805,141 +1801,138 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="15" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A20" s="16">
+    <row r="20" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>93</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="2">
         <v>10</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="L20" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="15" customFormat="1" ht="42" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
+    </row>
+    <row r="21" spans="1:13" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>95</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" s="16" t="s">
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="J21" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="L21" s="14" t="s">
+      <c r="L21" s="6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="28" x14ac:dyDescent="0.2">
-      <c r="A22" s="16">
+    <row r="22" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
         <v>96</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="16" t="s">
+      <c r="G22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="56" x14ac:dyDescent="0.2">
-      <c r="A23" s="19">
+    <row r="23" spans="1:13" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>98</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="19" t="s">
+      <c r="G23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="66" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>107</v>
       </c>
@@ -1971,154 +1964,219 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="56" x14ac:dyDescent="0.2">
-      <c r="A25" s="19">
+    <row r="25" spans="1:13" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>118</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="19" t="s">
+      <c r="G25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="2">
         <v>11</v>
       </c>
-      <c r="J25" s="20" t="s">
+      <c r="J25" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="L25" s="12" t="s">
+      <c r="L25" s="13" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="56" x14ac:dyDescent="0.2">
-      <c r="A26" s="16">
+    <row r="26" spans="1:13" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
         <v>119</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="16" t="s">
+      <c r="G26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I26" s="16">
+      <c r="I26" s="2">
         <v>11</v>
       </c>
-      <c r="J26" s="17" t="s">
+      <c r="J26" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K26" s="15"/>
-      <c r="L26" s="12" t="s">
+      <c r="L26" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="1:13" ht="70" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
+    </row>
+    <row r="27" spans="1:13" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="19" t="s">
+      <c r="G27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I27" s="22"/>
-      <c r="J27" s="20" t="s">
+      <c r="J27" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="15" customFormat="1" ht="70" x14ac:dyDescent="0.2">
-      <c r="A28" s="17">
+    <row r="28" spans="1:13" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
         <v>200</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="17" t="s">
+      <c r="H28" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="17" t="s">
+      <c r="J28" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="15" customFormat="1" ht="70" x14ac:dyDescent="0.2">
-      <c r="A29" s="17">
+    <row r="29" spans="1:13" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
         <v>201</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="17" t="s">
+      <c r="J29" s="6" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>109</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="M30" s="15">
+        <v>44076</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>112</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="M31" s="15">
+        <v>44076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>